<commit_message>
Export imported data from Excel file into JSON
</commit_message>
<xml_diff>
--- a/03-excel-spreadsheet/input/yumbo.xlsx
+++ b/03-excel-spreadsheet/input/yumbo.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="tasks" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="invoicing" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="invoicing periods" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="task bounds" sheetId="3" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="92">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -243,6 +244,60 @@
   </si>
   <si>
     <t xml:space="preserve">2025-08-17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-06-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-06-06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-06-13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-06-16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-06-23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-03-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-03-05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-05-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-05-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-03-01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-03-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-08-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-08-08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-08-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-08-15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-08-18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-08-22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-08-25</t>
   </si>
 </sst>
 </file>
@@ -337,7 +392,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -355,6 +410,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -739,8 +802,8 @@
   </sheetPr>
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -853,6 +916,305 @@
       </c>
       <c r="C10" s="6" t="s">
         <v>73</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C25"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H30" activeCellId="0" sqref="H30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>